<commit_message>
Update README to describe workflow and minor modifications to main dataset
</commit_message>
<xml_diff>
--- a/data/Colorado-Municipal-Water-Providers.xlsx
+++ b/data/Colorado-Municipal-Water-Providers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -7107,8 +7107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7534,11 +7534,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X531"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26911,7 +26911,7 @@
       </c>
       <c r="X283" s="90"/>
     </row>
-    <row r="284" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A284" s="78" t="s">
         <v>919</v>
       </c>
@@ -51532,7 +51532,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51643,7 +51643,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>